<commit_message>
CMA Compliance small template fix
</commit_message>
<xml_diff>
--- a/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.6.xlsx
+++ b/Projects/CCBOTTLERSUS/CMA/Data/CMA Compliance Template v0.6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -292,7 +292,7 @@
     <t>Vitamin Water Active Pump It 15.2 FL OZ PET,Vitamin Water Active Werk It 15.2 FL OZ PET,Vitamin Water Active Move It 15.2 FL OZ PET</t>
   </si>
   <si>
-    <t>MONSTER COFFEE+ENERGY </t>
+    <t>MONSTER COFFEE+ENERGY</t>
   </si>
   <si>
     <t>Coffee</t>
@@ -876,15 +876,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1074240</xdr:colOff>
+      <xdr:colOff>1100880</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -893,8 +893,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="7857360" cy="6349680"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="7914240" cy="6349320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -921,15 +921,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1074240</xdr:colOff>
+      <xdr:colOff>1100880</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -938,8 +938,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="7857360" cy="6349680"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="7914240" cy="6349320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -966,15 +966,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
+      <xdr:colOff>54000</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1074240</xdr:colOff>
+      <xdr:colOff>1100880</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>75960</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -983,8 +983,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="7857360" cy="6349680"/>
+          <a:off x="54000" y="0"/>
+          <a:ext cx="7914240" cy="6349320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1024,13 +1024,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.8825910931174"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.7044534412955"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.21052631578947"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.5627530364373"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1312,7 +1312,7 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="4" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="46.5951417004049"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="46.919028340081"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="4" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1013" min="4" style="4" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1022" min="1014" style="5" width="9.10526315789474"/>
@@ -1359,24 +1359,24 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.9878542510121"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="29.5668016194332"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -1915,17 +1915,17 @@
   </sheetPr>
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.7732793522267"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0283400809717"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.2388663967611"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.39271255060729"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.5991902834008"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.21052631578947"/>
   </cols>
   <sheetData>
@@ -2813,9 +2813,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.8502024291498"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>